<commit_message>
fix saving and change to gpt-4
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -31,19 +31,19 @@
     <t>Other sustainability data:</t>
   </si>
   <si>
-    <t>The text discusses how the Investment Manager incorporates ESG factors into its investment process.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> It uses a proprietary scoring model to assess ESG risks and opportunities, considering factors such as political stability, corruption, climate change vulnerability, and natural resource management.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The Investment Manager also promotes environmental and social characteristics by excluding certain industries and engaging with issuers.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> It seeks to avoid companies involved in controversial weapons, tobacco, palm oil production, and thermal coal mining.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Additionally, the Investment Manager integrates ESG factors into its fundamental analysis, believing that they are linked to competitive strengths and the sustainability of investments.</t>
+    <t>The Investment Manager integrates ESG factors into its investment process, using a proprietary scoring model that incorporates data from third-party vendors and publicly available sources.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The model considers governance factors such as political stability, government effectiveness, institutional strength, corruption levels, and rule of law.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Environmental factors include vulnerability to climate change and natural disasters, energy transition risk, energy security, and natural resource management.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Social factors include living standards, income inequality, human rights, poverty, gender inequality, healthcare and education access, personal safety, housing, food security, demographic change, employment rights, and social cohesion.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The Investment Manager also excludes companies involved in the manufacturing of controversial weapons, violating global norms, or deriving significant revenue from tobacco-related businesses, palm oil production, thermal coal mining, or thermal coal-related power generation.</t>
   </si>
 </sst>
 </file>
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -399,26 +399,31 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>